<commit_message>
feat: marcação no excel das linhas selecionadas
</commit_message>
<xml_diff>
--- a/filtered_data.xlsx
+++ b/filtered_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="63">
   <si>
     <t>id</t>
   </si>
@@ -46,103 +46,88 @@
     <t>conta</t>
   </si>
   <si>
-    <t>2024-10-03 00:00:00</t>
+    <t>2024-10-04 00:00:00</t>
   </si>
   <si>
     <t>2024-10-08 00:00:00</t>
   </si>
   <si>
-    <t>2024-10-11 00:00:00</t>
-  </si>
-  <si>
-    <t>210201010037</t>
-  </si>
-  <si>
-    <t>2024-10-15 00:00:00</t>
-  </si>
-  <si>
-    <t>2024-10-16 00:00:00</t>
-  </si>
-  <si>
-    <t>2024-10-21 00:00:00</t>
+    <t>2024-10-18 00:00:00</t>
+  </si>
+  <si>
+    <t>2024-10-22 00:00:00</t>
+  </si>
+  <si>
+    <t>2024-10-23 00:00:00</t>
   </si>
   <si>
     <t>2024-10-25 00:00:00</t>
   </si>
   <si>
-    <t>VLR. DOC. N. 902145160  ESCR.CENTRAL ARREC.DISTR.- ECAD</t>
-  </si>
-  <si>
-    <t>VLR. NF. N. 902145184  ESCR.CENTRAL ARREC.DISTR.- ECAD</t>
-  </si>
-  <si>
-    <t>N/PGTO. DUPL. N. 9021433525  ESCR.CENTRAL ARREC.DISTR.- ECAD</t>
-  </si>
-  <si>
-    <t>N/PGTO. DUPL. N. 902145160  ESCR.CENTRAL ARREC.DISTR.- ECAD</t>
-  </si>
-  <si>
-    <t>N/PGTO. DUPL. N. 902145184  ESCR.CENTRAL</t>
-  </si>
-  <si>
-    <t>nan ARREC.DISTR.- ECAD</t>
-  </si>
-  <si>
-    <t>VLR. DOC. N. 9021451848  ESCR.CENTRAL ARREC.DISTR.- ECAD</t>
-  </si>
-  <si>
-    <t>VLR. DOC. N. 9021460441  ESCR.CENTRAL ARREC.DISTR.- ECAD</t>
-  </si>
-  <si>
-    <t>N/PGTO. DUPL. N.  9021460441 ESCR.CENTRAL ARREC.DISTR.- ECAD</t>
-  </si>
-  <si>
-    <t>VLR. DOC. N.  9021462012 ESCR.CENTRAL ARREC.DISTR.- ECAD</t>
-  </si>
-  <si>
-    <t>VLR. DOC. N.  9021462013 ESCR.CENTRAL ARREC.DISTR.- ECAD</t>
-  </si>
-  <si>
-    <t>4558</t>
-  </si>
-  <si>
-    <t>4612</t>
+    <t>VLR. NF. N. 570  DEUCHER RESTAURANTE EIRELI</t>
+  </si>
+  <si>
+    <t>VLR. NF. N. 569  DEUCHER RESTAURANTE EIRELI</t>
+  </si>
+  <si>
+    <t>N/PGTO. NF. N. 569  DEUCHER RESTAURANTE EIRELI</t>
+  </si>
+  <si>
+    <t>N/PGTO. NF. N. 570  DEUCHER RESTAURANTE EIRELI</t>
+  </si>
+  <si>
+    <t>VLR. NF. N. 576  DEUCHER RESTAURANTE EIRELI</t>
+  </si>
+  <si>
+    <t>N/PGTO. NF. N. 576  DEUCHER RESTAURANTE EIRELI</t>
+  </si>
+  <si>
+    <t>VLR. NF. N. 577  DEUCHER RESTAURANTE EIRELI</t>
+  </si>
+  <si>
+    <t>VLR. NF. N. 578  DEUCHER RESTAURANTE EIRELI</t>
+  </si>
+  <si>
+    <t>VLR. NF. N. 579  DEUCHER RESTAURANTE EIRELI</t>
+  </si>
+  <si>
+    <t>VLR. NF. N. 580  DEUCHER RESTAURANTE EIRELI</t>
+  </si>
+  <si>
+    <t>VLR. NF. N. 581  DEUCHER RESTAURANTE EIRELI</t>
+  </si>
+  <si>
+    <t>N/PGTO. NF. N. 577  DEUCHER RESTAURANTE EIRELI</t>
+  </si>
+  <si>
+    <t>N/PGTO. NF. N. 578  DEUCHER RESTAURANTE EIRELI</t>
+  </si>
+  <si>
+    <t>N/PGTO. NF. N. 579  DEUCHER RESTAURANTE EIRELI</t>
+  </si>
+  <si>
+    <t>N/PGTO. NF. N. 580  DEUCHER RESTAURANTE EIRELI</t>
+  </si>
+  <si>
+    <t>N/PGTO. NF. N. 581  DEUCHER RESTAURANTE EIRELI</t>
+  </si>
+  <si>
+    <t>4572</t>
   </si>
   <si>
     <t>4828</t>
   </si>
   <si>
-    <t>4809</t>
-  </si>
-  <si>
-    <t>4780</t>
-  </si>
-  <si>
-    <t>4822</t>
-  </si>
-  <si>
-    <t>4938</t>
-  </si>
-  <si>
-    <t>5027</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>151</t>
-  </si>
-  <si>
-    <t>217</t>
-  </si>
-  <si>
-    <t>275</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>5</t>
+    <t>4867</t>
+  </si>
+  <si>
+    <t>4962</t>
+  </si>
+  <si>
+    <t>4974</t>
+  </si>
+  <si>
+    <t>5063</t>
   </si>
   <si>
     <t>10</t>
@@ -151,34 +136,64 @@
     <t>12</t>
   </si>
   <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
     <t>14</t>
   </si>
   <si>
-    <t>398.19</t>
-  </si>
-  <si>
-    <t>7875</t>
-  </si>
-  <si>
-    <t>6150</t>
-  </si>
-  <si>
-    <t>1919.82</t>
-  </si>
-  <si>
-    <t>Transporte da página anterior:</t>
-  </si>
-  <si>
-    <t>10125</t>
-  </si>
-  <si>
-    <t>2700</t>
-  </si>
-  <si>
-    <t>1409.04</t>
-  </si>
-  <si>
-    <t>9393.6</t>
+    <t>16</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>25165</t>
+  </si>
+  <si>
+    <t>16550</t>
+  </si>
+  <si>
+    <t>14423</t>
+  </si>
+  <si>
+    <t>2388</t>
+  </si>
+  <si>
+    <t>81640</t>
+  </si>
+  <si>
+    <t>6540</t>
+  </si>
+  <si>
+    <t>50220</t>
+  </si>
+  <si>
+    <t>6960</t>
   </si>
   <si>
     <t>C</t>
@@ -187,7 +202,7 @@
     <t>D</t>
   </si>
   <si>
-    <t>02437</t>
+    <t>02089</t>
   </si>
 </sst>
 </file>
@@ -211,12 +226,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -246,11 +267,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,7 +567,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -585,308 +607,428 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2">
-        <v>103</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="I2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="J2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3">
-        <v>104</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4">
-        <v>105</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" t="s">
-        <v>57</v>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
-        <v>106</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="I5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="J5" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
-        <v>107</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7">
-        <v>108</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" t="s">
-        <v>50</v>
-      </c>
-      <c r="I7" t="s">
-        <v>56</v>
-      </c>
-      <c r="J7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8">
-        <v>109</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" t="s">
-        <v>51</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="J8" t="s">
-        <v>57</v>
+      <c r="I8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
-        <v>110</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H9" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="I9" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="J9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10">
-        <v>111</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" t="s">
-        <v>49</v>
-      </c>
-      <c r="I10" t="s">
-        <v>55</v>
-      </c>
-      <c r="J10" t="s">
-        <v>57</v>
+      <c r="I10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
-        <v>112</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
         <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H11" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="I11" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="J11" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12">
-        <v>113</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" t="s">
-        <v>53</v>
-      </c>
-      <c r="I12" t="s">
-        <v>55</v>
-      </c>
-      <c r="J12" t="s">
-        <v>57</v>
+      <c r="F12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
-        <v>114</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
         <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" t="s">
-        <v>54</v>
+        <v>47</v>
+      </c>
+      <c r="G13" t="s">
+        <v>55</v>
       </c>
       <c r="I13" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="J13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" t="s">
         <v>57</v>
+      </c>
+      <c r="I15" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: save conciliated and non conciliated
</commit_message>
<xml_diff>
--- a/filtered_data.xlsx
+++ b/filtered_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="64">
   <si>
     <t>id</t>
   </si>
@@ -229,12 +229,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -264,11 +270,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,89 +612,95 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K2">
+      <c r="I2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3">
+      <c r="I3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" s="2">
         <v>1</v>
       </c>
     </row>
@@ -750,60 +763,64 @@
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I7" t="s">
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J7" t="s">
-        <v>63</v>
-      </c>
-      <c r="K7">
+      <c r="J7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E8" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I8" t="s">
-        <v>61</v>
-      </c>
-      <c r="J8" t="s">
-        <v>63</v>
-      </c>
-      <c r="K8">
+      <c r="I8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" s="2">
         <v>1</v>
       </c>
     </row>
@@ -837,118 +854,126 @@
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E10" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H10" t="s">
+      <c r="G10" s="2"/>
+      <c r="H10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I10" t="s">
-        <v>61</v>
-      </c>
-      <c r="J10" t="s">
-        <v>63</v>
-      </c>
-      <c r="K10">
+      <c r="I10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E11" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H11" t="s">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J11" t="s">
-        <v>63</v>
-      </c>
-      <c r="K11">
+      <c r="I11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K11" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E12" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H12" t="s">
+      <c r="G12" s="2"/>
+      <c r="H12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I12" t="s">
-        <v>61</v>
-      </c>
-      <c r="J12" t="s">
-        <v>63</v>
-      </c>
-      <c r="K12">
+      <c r="I12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K12" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E13" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I13" t="s">
-        <v>61</v>
-      </c>
-      <c r="J13" t="s">
-        <v>63</v>
-      </c>
-      <c r="K13">
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13" s="2">
         <v>1</v>
       </c>
     </row>
@@ -982,31 +1007,33 @@
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E15" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I15" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" t="s">
-        <v>63</v>
-      </c>
-      <c r="K15">
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K15" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1040,31 +1067,33 @@
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E17" t="s">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I17" t="s">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J17" t="s">
-        <v>63</v>
-      </c>
-      <c r="K17">
+      <c r="J17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K17" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: save unselect status to db
</commit_message>
<xml_diff>
--- a/filtered_data.xlsx
+++ b/filtered_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="64">
   <si>
     <t>id</t>
   </si>
@@ -612,65 +612,61 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K2" s="2">
-        <v>1</v>
+      <c r="I2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="2">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
+      <c r="H3" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3" s="2">
-        <v>1</v>
+      <c r="I3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -734,32 +730,34 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H6" t="s">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I6" t="s">
-        <v>61</v>
-      </c>
-      <c r="J6" t="s">
-        <v>63</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
+      <c r="I6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11">

</xml_diff>

<commit_message>
fix: order numerical values when i filter
</commit_message>
<xml_diff>
--- a/filtered_data.xlsx
+++ b/filtered_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="64">
   <si>
     <t>id</t>
   </si>
@@ -674,119 +674,127 @@
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
+      <c r="J5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H6" t="s">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I6" t="s">
-        <v>61</v>
-      </c>
-      <c r="J6" t="s">
-        <v>63</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
+      <c r="I6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I7" t="s">
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J7" t="s">
-        <v>63</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
+      <c r="J7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -852,235 +860,251 @@
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E10" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H10" t="s">
+      <c r="G10" s="2"/>
+      <c r="H10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I10" t="s">
-        <v>61</v>
-      </c>
-      <c r="J10" t="s">
-        <v>63</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
+      <c r="I10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E11" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H11" t="s">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J11" t="s">
-        <v>63</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
+      <c r="I11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E12" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H12" t="s">
+      <c r="G12" s="2"/>
+      <c r="H12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I12" t="s">
-        <v>61</v>
-      </c>
-      <c r="J12" t="s">
-        <v>63</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
+      <c r="I12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E13" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I13" t="s">
-        <v>61</v>
-      </c>
-      <c r="J13" t="s">
-        <v>63</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E14" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I14" t="s">
-        <v>61</v>
-      </c>
-      <c r="J14" t="s">
-        <v>63</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E15" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I15" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" t="s">
-        <v>63</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E16" t="s">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I16" t="s">
-        <v>61</v>
-      </c>
-      <c r="J16" t="s">
-        <v>63</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E17" t="s">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I17" t="s">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J17" t="s">
-        <v>63</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
+      <c r="J17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: change conciliated collor on excel
</commit_message>
<xml_diff>
--- a/filtered_data.xlsx
+++ b/filtered_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="64">
   <si>
     <t>id</t>
   </si>
@@ -238,7 +238,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFD8E4BC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -767,344 +767,322 @@
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="2">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
+      <c r="E7" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" t="s">
         <v>55</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2" t="s">
+      <c r="I7" t="s">
         <v>62</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K7" s="2">
-        <v>1</v>
+      <c r="J7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="2">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
+      <c r="E8" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
+      <c r="H8" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K8" s="2">
-        <v>1</v>
+      <c r="I8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="2">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
+      <c r="E9" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
+      <c r="H9" t="s">
         <v>57</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K9" s="2">
-        <v>1</v>
+      <c r="I9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="2">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
+      <c r="E10" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
+      <c r="H10" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K10" s="2">
-        <v>1</v>
+      <c r="I10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="2">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
+      <c r="E11" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2" t="s">
+      <c r="H11" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K11" s="2">
-        <v>1</v>
+      <c r="I11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" t="s">
+        <v>63</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="2">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
+      <c r="E12" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2" t="s">
+      <c r="H12" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K12" s="2">
-        <v>1</v>
+      <c r="I12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="2">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
+      <c r="E13" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K13" s="2">
-        <v>1</v>
+      <c r="I13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="2">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
+      <c r="E14" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" t="s">
         <v>57</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1</v>
+      <c r="I14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="2">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
+      <c r="E15" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" t="s">
         <v>58</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K15" s="2">
-        <v>1</v>
+      <c r="I15" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" t="s">
+        <v>63</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="2">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2" t="s">
+      <c r="E16" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" t="s">
         <v>59</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K16" s="2">
-        <v>1</v>
+      <c r="I16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" t="s">
+        <v>63</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="2">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2" t="s">
+      <c r="E17" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" t="s">
         <v>60</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2" t="s">
+      <c r="I17" t="s">
         <v>62</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K17" s="2">
-        <v>1</v>
+      <c r="J17" t="s">
+        <v>63</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: table foot sum D and C
</commit_message>
<xml_diff>
--- a/filtered_data.xlsx
+++ b/filtered_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="64">
   <si>
     <t>id</t>
   </si>
@@ -767,90 +767,96 @@
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I7" t="s">
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J7" t="s">
-        <v>63</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
+      <c r="J7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E8" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I8" t="s">
-        <v>61</v>
-      </c>
-      <c r="J8" t="s">
-        <v>63</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
+      <c r="I8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E9" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H9" t="s">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I9" t="s">
-        <v>61</v>
-      </c>
-      <c r="J9" t="s">
-        <v>63</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
+      <c r="I9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -883,32 +889,34 @@
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E11" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H11" t="s">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J11" t="s">
-        <v>63</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
+      <c r="I11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -941,32 +949,34 @@
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E13" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I13" t="s">
-        <v>61</v>
-      </c>
-      <c r="J13" t="s">
-        <v>63</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1028,61 +1038,65 @@
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E16" t="s">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I16" t="s">
-        <v>61</v>
-      </c>
-      <c r="J16" t="s">
-        <v>63</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E17" t="s">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I17" t="s">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J17" t="s">
-        <v>63</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
+      <c r="J17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>